<commit_message>
gitkraken was slow to notice some changes, 2nd attempt
</commit_message>
<xml_diff>
--- a/result_data/cat_costume_results.xlsx
+++ b/result_data/cat_costume_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike Bahns\Desktop\ECE523\PROJECT\ece523\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike Bahns\Desktop\ECE523\PROJECT\ece523\result_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFED305-675A-4870-9B43-44B913AF9931}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4E9628-CF80-425D-B23D-65FCBC7E0A2B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="16815" windowHeight="18165" xr2:uid="{4C5CF025-BFDF-493A-B9AA-9C9EC3A096F4}"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="16815" windowHeight="18165" xr2:uid="{4C5CF025-BFDF-493A-B9AA-9C9EC3A096F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>ulx</t>
   </si>
@@ -45,7 +45,10 @@
     <t>% coverage</t>
   </si>
   <si>
-    <t>%cat factor</t>
+    <t>high-contrast</t>
+  </si>
+  <si>
+    <t>low-contrast</t>
   </si>
 </sst>
 </file>
@@ -53,7 +56,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -89,7 +92,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -185,7 +188,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12548381452318461"/>
+          <c:y val="0.14396892511181789"/>
+          <c:w val="0.78904330708661419"/>
+          <c:h val="0.68367474184235288"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -198,7 +211,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>%cat factor</c:v>
+                  <c:v>high-contrast</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -285,6 +298,105 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B817-427C-968E-BDF23B40F4B2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>low-contrast</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$8:$G$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.87890625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.44140625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.515625</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.78515625</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>6.25</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>7.91015625</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>9.765625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$8:$I$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>39.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BF23-4221-A75C-84C339F850EE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -546,6 +658,47 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.65890201224846889"/>
+          <c:y val="0.63651562210598456"/>
+          <c:w val="0.21887576552930885"/>
+          <c:h val="0.13100526370804422"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1484,10 +1637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3339FCF-FA4F-479D-8EA8-CA7294101561}">
-  <dimension ref="B7:H15"/>
+  <dimension ref="B7:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1497,7 +1650,7 @@
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -1519,8 +1672,11 @@
       <c r="H7" t="s">
         <v>6</v>
       </c>
+      <c r="I7" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>0.184</v>
       </c>
@@ -1534,19 +1690,22 @@
         <v>3</v>
       </c>
       <c r="F8" s="1">
-        <f>E8</f>
+        <f t="shared" ref="F8:F15" si="0">E8</f>
         <v>3</v>
       </c>
       <c r="G8" s="2">
-        <f>100*E8*F8/(32*32)</f>
+        <f t="shared" ref="G8:G15" si="1">100*E8*F8/(32*32)</f>
         <v>0.87890625</v>
       </c>
       <c r="H8">
-        <f>100*B8</f>
+        <f t="shared" ref="H8:H15" si="2">100*B8</f>
         <v>18.399999999999999</v>
       </c>
+      <c r="I8">
+        <v>11</v>
+      </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>0.26500000000000001</v>
       </c>
@@ -1560,19 +1719,22 @@
         <v>4</v>
       </c>
       <c r="F9" s="1">
-        <f>E9</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G9" s="2">
-        <f>100*E9*F9/(32*32)</f>
+        <f t="shared" si="1"/>
         <v>1.5625</v>
       </c>
       <c r="H9">
-        <f>100*B9</f>
+        <f t="shared" si="2"/>
         <v>26.5</v>
       </c>
+      <c r="I9">
+        <v>16.7</v>
+      </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>0.35599999999999998</v>
       </c>
@@ -1586,19 +1748,22 @@
         <v>5</v>
       </c>
       <c r="F10" s="1">
-        <f>E10</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G10" s="2">
-        <f>100*E10*F10/(32*32)</f>
+        <f t="shared" si="1"/>
         <v>2.44140625</v>
       </c>
       <c r="H10">
-        <f>100*B10</f>
+        <f t="shared" si="2"/>
         <v>35.6</v>
       </c>
+      <c r="I10">
+        <v>21.2</v>
+      </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>0.40799999999999997</v>
       </c>
@@ -1612,19 +1777,22 @@
         <v>6</v>
       </c>
       <c r="F11" s="1">
-        <f>E11</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="G11" s="2">
-        <f>100*E11*F11/(32*32)</f>
+        <f t="shared" si="1"/>
         <v>3.515625</v>
       </c>
       <c r="H11">
-        <f>100*B11</f>
+        <f t="shared" si="2"/>
         <v>40.799999999999997</v>
       </c>
+      <c r="I11">
+        <v>26.1</v>
+      </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>0.441</v>
       </c>
@@ -1638,19 +1806,22 @@
         <v>7</v>
       </c>
       <c r="F12" s="1">
-        <f>E12</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="G12" s="2">
-        <f>100*E12*F12/(32*32)</f>
+        <f t="shared" si="1"/>
         <v>4.78515625</v>
       </c>
       <c r="H12">
-        <f>100*B12</f>
+        <f t="shared" si="2"/>
         <v>44.1</v>
       </c>
+      <c r="I12">
+        <v>32.299999999999997</v>
+      </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>0.50800000000000001</v>
       </c>
@@ -1664,19 +1835,22 @@
         <v>8</v>
       </c>
       <c r="F13" s="1">
-        <f>E13</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G13" s="1">
-        <f>100*E13*F13/(32*32)</f>
+        <f t="shared" si="1"/>
         <v>6.25</v>
       </c>
       <c r="H13">
-        <f>100*B13</f>
+        <f t="shared" si="2"/>
         <v>50.8</v>
       </c>
+      <c r="I13">
+        <v>39.799999999999997</v>
+      </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>0.57499999999999996</v>
       </c>
@@ -1690,19 +1864,22 @@
         <v>9</v>
       </c>
       <c r="F14" s="1">
-        <f>E14</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="G14" s="1">
-        <f>100*E14*F14/(32*32)</f>
+        <f t="shared" si="1"/>
         <v>7.91015625</v>
       </c>
       <c r="H14">
-        <f>100*B14</f>
+        <f t="shared" si="2"/>
         <v>57.499999999999993</v>
       </c>
+      <c r="I14">
+        <v>40.700000000000003</v>
+      </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>0.59799999999999998</v>
       </c>
@@ -1716,16 +1893,19 @@
         <v>10</v>
       </c>
       <c r="F15" s="1">
-        <f>E15</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G15" s="1">
-        <f>100*E15*F15/(32*32)</f>
+        <f t="shared" si="1"/>
         <v>9.765625</v>
       </c>
       <c r="H15">
-        <f>100*B15</f>
+        <f t="shared" si="2"/>
         <v>59.8</v>
+      </c>
+      <c r="I15">
+        <v>41.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to cat_disguise_demo, and graph
</commit_message>
<xml_diff>
--- a/result_data/cat_costume_results.xlsx
+++ b/result_data/cat_costume_results.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike Bahns\Desktop\ECE523\PROJECT\ece523\result_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4E9628-CF80-425D-B23D-65FCBC7E0A2B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D0E472-8A25-4306-A11D-CE8776D7A3B3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="16815" windowHeight="18165" xr2:uid="{4C5CF025-BFDF-493A-B9AA-9C9EC3A096F4}"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="22440" windowHeight="18135" xr2:uid="{4C5CF025-BFDF-493A-B9AA-9C9EC3A096F4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="costumes" sheetId="1" r:id="rId1"/>
+    <sheet name="disguises" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>ulx</t>
   </si>
@@ -39,9 +40,6 @@
     <t>h</t>
   </si>
   <si>
-    <t>cat factor</t>
-  </si>
-  <si>
     <t>% coverage</t>
   </si>
   <si>
@@ -49,6 +47,27 @@
   </si>
   <si>
     <t>low-contrast</t>
+  </si>
+  <si>
+    <t>pixels covered</t>
+  </si>
+  <si>
+    <t>best</t>
+  </si>
+  <si>
+    <t>ave prog reduction</t>
+  </si>
+  <si>
+    <t>average % reduction</t>
+  </si>
+  <si>
+    <t>high cont</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>high</t>
   </si>
 </sst>
 </file>
@@ -133,7 +152,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -147,13 +166,17 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Cat Costume Effectiveness vs. %</a:t>
+              <a:t>COSTUME Effectiveness </a:t>
             </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Pixels Covered</a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>vs. % PIXELS Covered</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -170,7 +193,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -194,9 +217,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.12548381452318461"/>
-          <c:y val="0.14396892511181789"/>
+          <c:y val="0.19511048790134111"/>
           <c:w val="0.78904330708661419"/>
-          <c:h val="0.68367474184235288"/>
+          <c:h val="0.63253327580627761"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -207,7 +230,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$7</c:f>
+              <c:f>costumes!$L$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -217,7 +240,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -230,10 +253,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$8:$G$15</c:f>
+              <c:f>costumes!$J$8:$J$21</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>0.87890625</c:v>
                 </c:pt>
@@ -257,16 +280,34 @@
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
                   <c:v>9.765625</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>11.81640625</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>14.0625</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>15.234375</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>16.40625</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>17.578125</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>18.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$8:$H$15</c:f>
+              <c:f>costumes!$L$8:$L$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>18.399999999999999</c:v>
                 </c:pt>
@@ -290,6 +331,24 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>59.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>61.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>78.600000000000009</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>92.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>94.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -306,7 +365,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$7</c:f>
+              <c:f>costumes!$N$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -316,7 +375,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -329,10 +388,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$8:$G$15</c:f>
+              <c:f>costumes!$J$8:$J$21</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>0.87890625</c:v>
                 </c:pt>
@@ -356,16 +415,34 @@
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
                   <c:v>9.765625</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>11.81640625</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>14.0625</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>15.234375</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>16.40625</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>17.578125</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>18.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$8:$I$15</c:f>
+              <c:f>costumes!$N$8:$N$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>11</c:v>
                 </c:pt>
@@ -379,16 +456,34 @@
                   <c:v>26.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32.299999999999997</c:v>
+                  <c:v>32.300000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>39.799999999999997</c:v>
+                  <c:v>39.800000000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40.700000000000003</c:v>
+                  <c:v>40.699999999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41.1</c:v>
+                  <c:v>41.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>62.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>72.3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>73.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>80.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>86.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>89</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -415,6 +510,7 @@
         <c:axId val="694709832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="20"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -439,7 +535,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -452,14 +548,9 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>%</a:t>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>% Image Pixels Covered by Cat Costume</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Image Pixels Covered by Cat Costume</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -476,7 +567,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -500,9 +591,9 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -561,7 +652,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -574,7 +665,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" b="1"/>
                   <a:t>Cat Costume Success %</a:t>
                 </a:r>
               </a:p>
@@ -593,7 +684,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -617,9 +708,9 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -659,15 +750,15 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="t"/>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.65890201224846889"/>
-          <c:y val="0.63651562210598456"/>
-          <c:w val="0.21887576552930885"/>
-          <c:h val="0.13100526370804422"/>
+          <c:x val="0.26154068241469819"/>
+          <c:y val="0.72997562837768859"/>
+          <c:w val="0.47788517151816018"/>
+          <c:h val="5.6667067690643939E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -712,7 +803,501 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Effectiveness of Cat Disguise </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>vs. Number of Pixels</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>disguises!$G$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>average % reduction</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>disguises!$D$14:$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>disguises!$G$14:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>21.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35.699999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>49.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>51.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EED6-4DCF-B5C6-7EEAD2FEC14C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="603426232"/>
+        <c:axId val="603430496"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="603426232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Number of Pixels Covered (out of 3x3)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="603430496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="603430496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Average % Cat Probability Reduction</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="3.0555555555555555E-2"/>
+              <c:y val="0.19894681437634676"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="603426232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -783,8 +1368,48 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -795,7 +1420,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -811,25 +1436,25 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="bg1"/>
+        <a:schemeClr val="lt1"/>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
@@ -841,7 +1466,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -849,11 +1474,11 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -885,35 +1510,45 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -925,22 +1560,26 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -970,15 +1609,13 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -988,7 +1625,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -997,7 +1634,43 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
@@ -1007,65 +1680,125 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1078,54 +1811,17 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -1135,8 +1831,8 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
+  </cs:seriesLine>
+  <cs:title>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -1146,66 +1842,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1214,14 +1851,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1235,14 +1871,106 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1251,15 +1979,146 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -1270,11 +2129,307 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1287,14 +2442,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1303,15 +2452,56 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>461962</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>493059</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>123265</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>71437</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>147636</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E8F7A09-AC1D-40C5-ABB2-4BCA5F4C104F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1319,7 +2509,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E8F7A09-AC1D-40C5-ABB2-4BCA5F4C104F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89A7BE37-ECD0-43B6-A6F7-8605A93FF99D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1637,275 +2827,672 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3339FCF-FA4F-479D-8EA8-CA7294101561}">
-  <dimension ref="B7:I15"/>
+  <dimension ref="B6:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="6" width="9.140625" style="1"/>
-    <col min="7" max="7" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" style="1" customWidth="1"/>
+    <col min="12" max="13" width="9.140625" style="1"/>
+    <col min="14" max="14" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>4</v>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H7" t="s">
+      <c r="N7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="1" t="s">
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>0.184</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="D8" s="1">
+        <v>28</v>
+      </c>
+      <c r="E8" s="1">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1">
+        <v>3</v>
+      </c>
+      <c r="J8" s="2">
+        <f>100*G8*F8/(32*32)</f>
+        <v>0.87890625</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="1">
+        <f t="shared" ref="L8:L15" si="0">100*B8</f>
+        <v>18.399999999999999</v>
+      </c>
+      <c r="N8" s="1">
+        <f>100*C8</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="D9" s="1">
+        <v>24</v>
+      </c>
+      <c r="E9" s="1">
         <v>7</v>
       </c>
+      <c r="F9" s="1">
+        <v>4</v>
+      </c>
+      <c r="G9" s="1">
+        <v>4</v>
+      </c>
+      <c r="J9" s="2">
+        <f>100*G9*F9/(32*32)</f>
+        <v>1.5625</v>
+      </c>
+      <c r="K9" s="2"/>
+      <c r="L9" s="1">
+        <f t="shared" si="0"/>
+        <v>26.5</v>
+      </c>
+      <c r="N9" s="1">
+        <f>100*C9</f>
+        <v>16.7</v>
+      </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>0.184</v>
-      </c>
-      <c r="C8" s="1">
-        <v>28</v>
-      </c>
-      <c r="D8" s="1">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="D10" s="1">
+        <v>23</v>
+      </c>
+      <c r="E10" s="1">
+        <v>6</v>
+      </c>
+      <c r="F10" s="1">
+        <v>5</v>
+      </c>
+      <c r="G10" s="1">
+        <v>5</v>
+      </c>
+      <c r="J10" s="2">
+        <f>100*G10*F10/(32*32)</f>
+        <v>2.44140625</v>
+      </c>
+      <c r="K10" s="2"/>
+      <c r="L10" s="1">
+        <f t="shared" si="0"/>
+        <v>35.6</v>
+      </c>
+      <c r="N10" s="1">
+        <f>100*C10</f>
+        <v>21.2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>0.40799999999999997</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="D11" s="1">
+        <v>23</v>
+      </c>
+      <c r="E11" s="1">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1">
+        <v>6</v>
+      </c>
+      <c r="G11" s="1">
+        <v>6</v>
+      </c>
+      <c r="J11" s="2">
+        <f>100*G11*F11/(32*32)</f>
+        <v>3.515625</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="L11" s="1">
+        <f t="shared" si="0"/>
+        <v>40.799999999999997</v>
+      </c>
+      <c r="N11" s="1">
+        <f>100*C11</f>
+        <v>26.1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>0.441</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="D12" s="1">
+        <v>22</v>
+      </c>
+      <c r="E12" s="1">
         <v>4</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F12" s="1">
+        <v>7</v>
+      </c>
+      <c r="G12" s="1">
+        <v>7</v>
+      </c>
+      <c r="J12" s="2">
+        <f>100*G12*F12/(32*32)</f>
+        <v>4.78515625</v>
+      </c>
+      <c r="K12" s="2"/>
+      <c r="L12" s="1">
+        <f t="shared" si="0"/>
+        <v>44.1</v>
+      </c>
+      <c r="N12" s="1">
+        <f>100*C12</f>
+        <v>32.300000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="D13" s="1">
+        <v>22</v>
+      </c>
+      <c r="E13" s="1">
+        <v>4</v>
+      </c>
+      <c r="F13" s="1">
+        <v>8</v>
+      </c>
+      <c r="G13" s="1">
+        <v>8</v>
+      </c>
+      <c r="J13" s="1">
+        <f>100*G13*F13/(32*32)</f>
+        <v>6.25</v>
+      </c>
+      <c r="L13" s="1">
+        <f t="shared" si="0"/>
+        <v>50.8</v>
+      </c>
+      <c r="N13" s="1">
+        <f>100*C13</f>
+        <v>39.800000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="D14" s="1">
+        <v>21</v>
+      </c>
+      <c r="E14" s="1">
         <v>3</v>
       </c>
-      <c r="F8" s="1">
-        <f t="shared" ref="F8:F15" si="0">E8</f>
+      <c r="F14" s="1">
+        <v>9</v>
+      </c>
+      <c r="G14" s="1">
+        <v>9</v>
+      </c>
+      <c r="J14" s="1">
+        <f>100*G14*F14/(32*32)</f>
+        <v>7.91015625</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" si="0"/>
+        <v>57.499999999999993</v>
+      </c>
+      <c r="N14" s="1">
+        <f>100*C14</f>
+        <v>40.699999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="D15" s="1">
+        <v>21</v>
+      </c>
+      <c r="E15" s="1">
         <v>3</v>
       </c>
-      <c r="G8" s="2">
-        <f t="shared" ref="G8:G15" si="1">100*E8*F8/(32*32)</f>
-        <v>0.87890625</v>
-      </c>
-      <c r="H8">
-        <f t="shared" ref="H8:H15" si="2">100*B8</f>
-        <v>18.399999999999999</v>
-      </c>
-      <c r="I8">
+      <c r="F15" s="1">
+        <v>10</v>
+      </c>
+      <c r="G15" s="1">
+        <v>10</v>
+      </c>
+      <c r="J15" s="1">
+        <f>100*G15*F15/(32*32)</f>
+        <v>9.765625</v>
+      </c>
+      <c r="L15" s="1">
+        <f t="shared" si="0"/>
+        <v>59.8</v>
+      </c>
+      <c r="N15" s="1">
+        <f>100*C15</f>
+        <v>41.099999999999994</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.622</v>
+      </c>
+      <c r="F16" s="1">
         <v>11</v>
       </c>
+      <c r="G16" s="1">
+        <v>11</v>
+      </c>
+      <c r="J16" s="1">
+        <f>100*G16*F16/(32*32)</f>
+        <v>11.81640625</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" ref="L16:L24" si="1">100*B16</f>
+        <v>61.8</v>
+      </c>
+      <c r="N16" s="1">
+        <f t="shared" ref="N16:N24" si="2">100*C16</f>
+        <v>62.2</v>
+      </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>0.26500000000000001</v>
-      </c>
-      <c r="C9" s="1">
-        <v>24</v>
-      </c>
-      <c r="D9" s="1">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.72299999999999998</v>
+      </c>
+      <c r="F17" s="1">
+        <v>12</v>
+      </c>
+      <c r="G17" s="1">
+        <v>12</v>
+      </c>
+      <c r="J17" s="1">
+        <f>100*G17*F17/(32*32)</f>
+        <v>14.0625</v>
+      </c>
+      <c r="L17" s="1">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="N17" s="1">
+        <f t="shared" si="2"/>
+        <v>72.3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="F18" s="1">
+        <v>13</v>
+      </c>
+      <c r="G18" s="1">
+        <v>12</v>
+      </c>
+      <c r="J18" s="1">
+        <f>100*G18*F18/(32*32)</f>
+        <v>15.234375</v>
+      </c>
+      <c r="L18" s="1">
+        <f t="shared" si="1"/>
+        <v>78.600000000000009</v>
+      </c>
+      <c r="N18" s="1">
+        <f t="shared" si="2"/>
+        <v>73.5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>0.91</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="F19" s="1">
+        <v>14</v>
+      </c>
+      <c r="G19" s="1">
+        <v>12</v>
+      </c>
+      <c r="J19" s="1">
+        <f>100*G19*F19/(32*32)</f>
+        <v>16.40625</v>
+      </c>
+      <c r="L19" s="1">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="N19" s="1">
+        <f t="shared" si="2"/>
+        <v>80.400000000000006</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="F20" s="1">
+        <v>15</v>
+      </c>
+      <c r="G20" s="1">
+        <v>12</v>
+      </c>
+      <c r="J20" s="1">
+        <f>100*G20*F20/(32*32)</f>
+        <v>17.578125</v>
+      </c>
+      <c r="L20" s="1">
+        <f t="shared" si="1"/>
+        <v>92.5</v>
+      </c>
+      <c r="N20" s="1">
+        <f t="shared" si="2"/>
+        <v>86.8</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="F21" s="1">
+        <v>16</v>
+      </c>
+      <c r="G21" s="1">
+        <v>12</v>
+      </c>
+      <c r="J21" s="1">
+        <f>100*G21*F21/(32*32)</f>
+        <v>18.75</v>
+      </c>
+      <c r="L21" s="1">
+        <f t="shared" si="1"/>
+        <v>94.8</v>
+      </c>
+      <c r="N21" s="1">
+        <f t="shared" si="2"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>0.94899999999999995</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.84899999999999998</v>
+      </c>
+      <c r="F22" s="1">
+        <v>17</v>
+      </c>
+      <c r="G22" s="1">
+        <v>12</v>
+      </c>
+      <c r="J22" s="1">
+        <f>100*G22*F22/(32*32)</f>
+        <v>19.921875</v>
+      </c>
+      <c r="L22" s="1">
+        <f t="shared" si="1"/>
+        <v>94.899999999999991</v>
+      </c>
+      <c r="N22" s="1">
+        <f t="shared" si="2"/>
+        <v>84.899999999999991</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8592226C-EC57-42BE-BA06-9004E6175827}">
+  <dimension ref="D13:G22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="G14">
+        <f>F14*100</f>
+        <v>21.2</v>
+      </c>
+    </row>
+    <row r="15" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <f>D14+1</f>
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="G15">
+        <f t="shared" ref="G15:G22" si="0">F15*100</f>
+        <v>35.699999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <f t="shared" ref="D16:D22" si="1">D15+1</f>
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>193</v>
+      </c>
+      <c r="F16">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>42.3</v>
+      </c>
+    </row>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="F9" s="1">
+      <c r="E17">
+        <v>195</v>
+      </c>
+      <c r="F17">
+        <v>0.49</v>
+      </c>
+      <c r="G17">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G9" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D18">
         <f t="shared" si="1"/>
-        <v>1.5625</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="2"/>
-        <v>26.5</v>
-      </c>
-      <c r="I9">
-        <v>16.7</v>
+        <v>5</v>
+      </c>
+      <c r="E18">
+        <v>199</v>
+      </c>
+      <c r="F18">
+        <v>0.495</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>49.5</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>0.35599999999999998</v>
-      </c>
-      <c r="C10" s="1">
-        <v>23</v>
-      </c>
-      <c r="D10" s="1">
+    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="E10" s="1">
-        <v>5</v>
-      </c>
-      <c r="F10" s="1">
+      <c r="E19">
+        <v>423</v>
+      </c>
+      <c r="F19">
+        <v>0.495</v>
+      </c>
+      <c r="G19">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="G10" s="2">
+        <v>49.5</v>
+      </c>
+    </row>
+    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D20">
         <f t="shared" si="1"/>
-        <v>2.44140625</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="2"/>
-        <v>35.6</v>
-      </c>
-      <c r="I10">
-        <v>21.2</v>
+        <v>7</v>
+      </c>
+      <c r="E20">
+        <v>487</v>
+      </c>
+      <c r="F20">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>51.9</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>0.40799999999999997</v>
-      </c>
-      <c r="C11" s="1">
-        <v>23</v>
-      </c>
-      <c r="D11" s="1">
-        <v>3</v>
-      </c>
-      <c r="E11" s="1">
-        <v>6</v>
-      </c>
-      <c r="F11" s="1">
+    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <v>503</v>
+      </c>
+      <c r="F21">
+        <v>0.52</v>
+      </c>
+      <c r="G21">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G11" s="2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D22">
         <f t="shared" si="1"/>
-        <v>3.515625</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="2"/>
-        <v>40.799999999999997</v>
-      </c>
-      <c r="I11">
-        <v>26.1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>0.441</v>
-      </c>
-      <c r="C12" s="1">
-        <v>22</v>
-      </c>
-      <c r="D12" s="1">
-        <v>4</v>
-      </c>
-      <c r="E12" s="1">
-        <v>7</v>
-      </c>
-      <c r="F12" s="1">
+        <v>9</v>
+      </c>
+      <c r="E22">
+        <v>511</v>
+      </c>
+      <c r="F22">
+        <v>0.502</v>
+      </c>
+      <c r="G22">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="G12" s="2">
-        <f t="shared" si="1"/>
-        <v>4.78515625</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="2"/>
-        <v>44.1</v>
-      </c>
-      <c r="I12">
-        <v>32.299999999999997</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>0.50800000000000001</v>
-      </c>
-      <c r="C13" s="1">
-        <v>22</v>
-      </c>
-      <c r="D13" s="1">
-        <v>4</v>
-      </c>
-      <c r="E13" s="1">
-        <v>8</v>
-      </c>
-      <c r="F13" s="1">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="G13" s="1">
-        <f t="shared" si="1"/>
-        <v>6.25</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="2"/>
-        <v>50.8</v>
-      </c>
-      <c r="I13">
-        <v>39.799999999999997</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="C14" s="1">
-        <v>21</v>
-      </c>
-      <c r="D14" s="1">
-        <v>3</v>
-      </c>
-      <c r="E14" s="1">
-        <v>9</v>
-      </c>
-      <c r="F14" s="1">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="G14" s="1">
-        <f t="shared" si="1"/>
-        <v>7.91015625</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="2"/>
-        <v>57.499999999999993</v>
-      </c>
-      <c r="I14">
-        <v>40.700000000000003</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>0.59799999999999998</v>
-      </c>
-      <c r="C15" s="1">
-        <v>21</v>
-      </c>
-      <c r="D15" s="1">
-        <v>3</v>
-      </c>
-      <c r="E15" s="1">
-        <v>10</v>
-      </c>
-      <c r="F15" s="1">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G15" s="1">
-        <f t="shared" si="1"/>
-        <v>9.765625</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="2"/>
-        <v>59.8</v>
-      </c>
-      <c r="I15">
-        <v>41.1</v>
+        <v>50.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>